<commit_message>
all tests passing, 0.6.0 parsing
</commit_message>
<xml_diff>
--- a/tests/030_eg-invalid.xlsx
+++ b/tests/030_eg-invalid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jamie\surround\VocExcel\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/rdflib/VocExcel/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9DB06A-306E-4FF6-9304-91DCC28C742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18356F1B-DCC7-A541-85D7-5D066CB43713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22845" yWindow="0" windowWidth="22740" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15660" yWindow="500" windowWidth="22740" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
@@ -1498,19 +1498,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="78.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="83.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="3"/>
+    <col min="1" max="1" width="78.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="83.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>132</v>
       </c>
@@ -1656,18 +1656,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>142</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>143</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>144</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
         <v>265</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>145</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>146</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>147</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>148</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>149</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>150</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>151</v>
       </c>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>152</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>153</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>154</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>155</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>156</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>157</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>158</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>159</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>160</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>161</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>162</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>163</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>164</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>165</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>166</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>167</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>168</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>169</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>170</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>171</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>172</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>173</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>174</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>175</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>32</v>
       </c>
@@ -2271,30 +2271,30 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="86.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="3"/>
+    <col min="1" max="1" width="15.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="86.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>21</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>40</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>51</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>132</v>
       </c>
@@ -2415,14 +2415,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
     </row>
-    <row r="18" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>31</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>28</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>26</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>29</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>30</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>92</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>25</v>
       </c>
@@ -2510,14 +2510,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>32</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>27</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>26</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>33</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>25</v>
       </c>
@@ -2582,19 +2582,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="59.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="47" style="16" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="16"/>
+    <col min="4" max="4" width="62.1640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="16" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>51</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>132</v>
       </c>
@@ -2745,18 +2745,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
         <v>120</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>31</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>82</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>83</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>84</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>85</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>86</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>32</v>
       </c>
@@ -2884,24 +2884,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="59.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="46" style="3" customWidth="1"/>
     <col min="4" max="4" width="74" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>132</v>
       </c>
@@ -3052,18 +3052,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>123</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>102</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>134</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
@@ -3205,9 +3205,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A16" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E20" r:id="rId3" display="http://cgi.vocabs.ga.gov.au/object?uri=http%3A//resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E20" r:id="rId2" display="http://cgi.vocabs.ga.gov.au/object?uri=http%3A//resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="A16" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3234,19 +3234,19 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -3334,13 +3334,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>130</v>
       </c>

</xml_diff>